<commit_message>
fixt tests with new python version info
</commit_message>
<xml_diff>
--- a/client/simulations/tests/pkdata_no_data.xlsx
+++ b/client/simulations/tests/pkdata_no_data.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uczmh2\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="11700"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Input Values" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
     <sheet name="Voltage Traces (Plot format)" sheetId="5" r:id="rId5"/>
     <sheet name="ApPredict version information" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -35,7 +30,7 @@
     <t>Created at</t>
   </si>
   <si>
-    <t>2022-03-09 18:16:00.581635</t>
+    <t>2022-12-12 18:30:04.186656</t>
   </si>
   <si>
     <t>Created by</t>
@@ -89,7 +84,7 @@
     <t>PK data file</t>
   </si>
   <si>
-    <t>d62260ab-d88d-4c10-9805-a2ae0c753b5b_pk_data.tsv</t>
+    <t>890c10d9-87a7-4b49-a798-3642e182b282_pk_data.tsv</t>
   </si>
   <si>
     <t>Notes</t>
@@ -131,8 +126,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,14 +173,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -232,7 +219,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,10 +251,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -299,7 +285,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -475,14 +460,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -498,7 +483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -506,7 +491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -514,7 +499,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -528,7 +513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
@@ -539,7 +524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -562,7 +547,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -570,7 +555,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -584,14 +569,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -620,14 +605,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -641,26 +626,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -671,12 +656,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>